<commit_message>
11 : 50 수정 중...
</commit_message>
<xml_diff>
--- a/기능명세(수정 중).xlsx
+++ b/기능명세(수정 중).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\602-01\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C60CAD-3751-40AD-8E90-EAC3DDB03F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221C723-5650-4D89-A0ED-4FCD94375CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5250" yWindow="720" windowWidth="18240" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>번호</t>
   </si>
@@ -111,6 +111,10 @@
   </si>
   <si>
     <t>전선아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정영훈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -455,6 +459,26 @@
         <charset val="129"/>
       </rPr>
       <t>코드로 만족도 설문조사 참여 가능.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채팅방</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>WebSocket을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 이용한 채팅방 기능. ( 방 만들기, 채팅방 참여 )</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -554,7 +578,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +699,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF38F8F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -696,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -936,6 +966,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -945,6 +984,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF38F8F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1219,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ46"/>
+  <dimension ref="A1:BJ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1286,13 +1330,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="65" t="s">
         <v>22</v>
@@ -1304,10 +1348,10 @@
       <c r="A8" s="68"/>
       <c r="B8" s="64"/>
       <c r="C8" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="58"/>
@@ -1317,10 +1361,10 @@
       <c r="A9" s="68"/>
       <c r="B9" s="64"/>
       <c r="C9" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="58"/>
@@ -1330,10 +1374,10 @@
       <c r="A10" s="70"/>
       <c r="B10" s="70"/>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E10" s="70"/>
       <c r="F10" s="55"/>
@@ -1343,10 +1387,10 @@
       <c r="A11" s="70"/>
       <c r="B11" s="70"/>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E11" s="70"/>
       <c r="F11" s="42"/>
@@ -1356,10 +1400,10 @@
       <c r="A12" s="70"/>
       <c r="B12" s="70"/>
       <c r="C12" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="70"/>
       <c r="F12" s="55"/>
@@ -1369,10 +1413,10 @@
       <c r="A13" s="70"/>
       <c r="B13" s="70"/>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="70"/>
       <c r="F13" s="42"/>
@@ -1383,13 +1427,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="65" t="s">
         <v>22</v>
@@ -1401,10 +1445,10 @@
       <c r="A15" s="68"/>
       <c r="B15" s="69"/>
       <c r="C15" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="58"/>
@@ -1414,10 +1458,10 @@
       <c r="A16" s="68"/>
       <c r="B16" s="69"/>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="58"/>
@@ -1427,10 +1471,10 @@
       <c r="A17" s="68"/>
       <c r="B17" s="69"/>
       <c r="C17" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E17" s="65"/>
       <c r="F17" s="58"/>
@@ -1440,10 +1484,10 @@
       <c r="A18" s="68"/>
       <c r="B18" s="69"/>
       <c r="C18" s="56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" s="65"/>
       <c r="F18" s="58"/>
@@ -1453,10 +1497,10 @@
       <c r="A19" s="68"/>
       <c r="B19" s="69"/>
       <c r="C19" s="56" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="65"/>
       <c r="F19" s="58"/>
@@ -1472,13 +1516,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="66" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F20" s="58"/>
       <c r="G20" s="7"/>
@@ -1487,10 +1531,10 @@
       <c r="A21" s="68"/>
       <c r="B21" s="60"/>
       <c r="C21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" s="65"/>
       <c r="F21" s="58"/>
@@ -1503,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="65"/>
       <c r="F22" s="58"/>
@@ -1514,13 +1558,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" s="65" t="s">
         <v>21</v>
@@ -1532,10 +1576,10 @@
       <c r="A24" s="68"/>
       <c r="B24" s="61"/>
       <c r="C24" s="79" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E24" s="65"/>
       <c r="F24" s="58"/>
@@ -1546,7 +1590,7 @@
       <c r="B25" s="70"/>
       <c r="C25" s="70"/>
       <c r="D25" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" s="70"/>
       <c r="F25" s="42"/>
@@ -1557,7 +1601,7 @@
       <c r="B26" s="70"/>
       <c r="C26" s="70"/>
       <c r="D26" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E26" s="70"/>
       <c r="F26" s="42"/>
@@ -1571,10 +1615,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E27" s="67" t="s">
         <v>22</v>
@@ -1586,10 +1630,10 @@
       <c r="A28" s="68"/>
       <c r="B28" s="57"/>
       <c r="C28" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E28" s="67"/>
       <c r="F28" s="58"/>
@@ -1599,10 +1643,10 @@
       <c r="A29" s="68"/>
       <c r="B29" s="57"/>
       <c r="C29" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E29" s="67"/>
       <c r="F29" s="58"/>
@@ -1671,13 +1715,13 @@
         <v>8</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D30" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="52" t="s">
         <v>65</v>
-      </c>
-      <c r="E30" s="52" t="s">
-        <v>64</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="36"/>
@@ -1748,7 +1792,7 @@
         <v>17</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E31" s="48" t="s">
         <v>20</v>
@@ -1822,7 +1866,7 @@
         <v>15</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E32" s="48" t="s">
         <v>21</v>
@@ -1896,7 +1940,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E33" s="52" t="s">
         <v>19</v>
@@ -1964,10 +2008,10 @@
         <v>10</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" s="71" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>18</v>
@@ -1978,33 +2022,70 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:62" ht="29.25" customHeight="1">
+    <row r="35" spans="1:62" ht="34.5" customHeight="1">
       <c r="A35" s="68"/>
       <c r="B35" s="59"/>
       <c r="C35" s="70"/>
       <c r="D35" s="43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E35" s="65"/>
       <c r="F35" s="6"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:62" ht="16.5">
-      <c r="A36" s="68"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:62" ht="16.5">
-      <c r="A37" s="68"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="29"/>
+    <row r="36" spans="1:62" s="47" customFormat="1" ht="69" customHeight="1">
+      <c r="A36" s="51">
+        <v>11</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="53"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="50"/>
+      <c r="AA36" s="50"/>
+      <c r="AB36" s="50"/>
+    </row>
+    <row r="37" spans="1:62" ht="24" customHeight="1">
+      <c r="A37" s="68">
+        <v>12</v>
+      </c>
+      <c r="B37" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>76</v>
+      </c>
       <c r="E37" s="65"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="74"/>
       <c r="G37" s="34"/>
       <c r="H37" s="35"/>
       <c r="I37" s="35"/>
@@ -2028,158 +2109,97 @@
       <c r="AA37" s="35"/>
       <c r="AB37" s="35"/>
     </row>
-    <row r="38" spans="1:62" s="47" customFormat="1" ht="69" customHeight="1">
-      <c r="A38" s="51">
-        <v>11</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="50"/>
-      <c r="S38" s="50"/>
-      <c r="T38" s="50"/>
-      <c r="U38" s="50"/>
-      <c r="V38" s="50"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="50"/>
-      <c r="Y38" s="50"/>
-      <c r="Z38" s="50"/>
-      <c r="AA38" s="50"/>
-      <c r="AB38" s="50"/>
-    </row>
-    <row r="39" spans="1:62" ht="24" customHeight="1">
-      <c r="A39" s="68">
-        <v>12</v>
-      </c>
-      <c r="B39" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="65"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
-      <c r="W39" s="35"/>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="35"/>
-    </row>
-    <row r="40" spans="1:62" ht="21.75" customHeight="1">
+    <row r="38" spans="1:62" ht="21.75" customHeight="1">
+      <c r="A38" s="72"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+    </row>
+    <row r="39" spans="1:62" ht="36" customHeight="1">
+      <c r="A39" s="72"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+    </row>
+    <row r="40" spans="1:62" ht="39" customHeight="1">
       <c r="A40" s="72"/>
       <c r="B40" s="72"/>
-      <c r="C40" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="75" t="s">
-        <v>77</v>
+      <c r="C40" s="70"/>
+      <c r="D40" s="76" t="s">
+        <v>80</v>
       </c>
       <c r="E40" s="72"/>
       <c r="F40" s="72"/>
     </row>
-    <row r="41" spans="1:62" ht="36" customHeight="1">
+    <row r="41" spans="1:62" ht="24" customHeight="1">
       <c r="A41" s="72"/>
       <c r="B41" s="72"/>
-      <c r="C41" s="73" t="s">
-        <v>89</v>
+      <c r="C41" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="D41" s="76" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E41" s="72"/>
       <c r="F41" s="72"/>
     </row>
-    <row r="42" spans="1:62" ht="39" customHeight="1">
-      <c r="A42" s="72"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-    </row>
-    <row r="43" spans="1:62" ht="24" customHeight="1">
-      <c r="A43" s="72"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-    </row>
-    <row r="44" spans="1:62" ht="59.25" customHeight="1">
-      <c r="A44" s="1">
+    <row r="42" spans="1:62" ht="59.25" customHeight="1">
+      <c r="A42" s="1">
         <v>13</v>
       </c>
-      <c r="B44" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="77" t="s">
+      <c r="B42" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
-    </row>
-    <row r="45" spans="1:62">
-      <c r="B45" s="38"/>
-    </row>
-    <row r="46" spans="1:62">
-      <c r="B46" s="38"/>
+      <c r="C42" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
+    </row>
+    <row r="43" spans="1:62" ht="33" customHeight="1">
+      <c r="A43" s="1">
+        <v>14</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="54"/>
+    </row>
+    <row r="44" spans="1:62">
+      <c r="B44" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="31">
     <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="E39:E43"/>
-    <mergeCell ref="F39:F43"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="F37:F41"/>
     <mergeCell ref="A7:A13"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="E7:E13"/>
@@ -2188,23 +2208,23 @@
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="E34:E35"/>
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E27:E29"/>
-    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="F27:F29"/>
-    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="F14:F19"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="F20:F22"/>
     <mergeCell ref="F23:F24"/>
-    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>